<commit_message>
fixed all issues in apis
</commit_message>
<xml_diff>
--- a/public/imports/enquiry_sample.xlsx
+++ b/public/imports/enquiry_sample.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>ClientName</t>
   </si>
@@ -47,13 +47,7 @@
     <t>BudgetFrom</t>
   </si>
   <si>
-    <t>BudgetFromUnit</t>
-  </si>
-  <si>
     <t>BudgetTo</t>
-  </si>
-  <si>
-    <t>BudgetToUnit</t>
   </si>
   <si>
     <t>AssingedTo</t>
@@ -96,15 +90,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,11 +426,9 @@
     <col min="14" max="14" width="15" customWidth="true" style="0"/>
     <col min="15" max="15" width="15" customWidth="true" style="0"/>
     <col min="16" max="16" width="15" customWidth="true" style="0"/>
-    <col min="17" max="17" width="15" customWidth="true" style="0"/>
-    <col min="18" max="18" width="15" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,47 +477,34 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <dataValidations count="11">
+  <dataValidations count="9">
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="D2:D1048576">
-      <formula1>"Rent, Buy"</formula1>
+      <formula1>"Rent, Buy,Both"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="E2:E1048576">
-      <formula1>"Commercial,Industrial,Residential,Land/Plot"</formula1>
+      <formula1>"Industrial,Commercial,Residential,Office &amp; Retail,Residential &amp; Commercial,Industrial,Residentia l&amp; Commercial,Industrial,Industrial,Industrial,Industrial"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="F2:F1048576">
-      <formula1>"Agriculture Land,Corporate House,Godown,NA Land,Pent House,Row House,Tenament,Villa,Basement,Industrial Shed,Flat,Bungalow"</formula1>
+      <formula1>"Flat,Vila/Bunglow,Land/Plot,Penthouse,Farmhouse,Office,Retail,Storage/industrial,Plot/Land"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="G2:G1048576">
-      <formula1>"2 BHK,3 BHK,Basement,Godown,Industrial Land,Industrial Shed,Land Or Plot,Office Space,Showroom/Shop Ground Floor,Showroom/Shop 1st Floor,Showroom/Shop 2nd Floor"</formula1>
+      <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,4+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="H2:H1048576">
-      <formula1>"2 BHK,3 BHK,Basement,Godown,Industrial Land,Industrial Shed,Land Or Plot,Office Space,Showroom/Shop Ground Floor,Showroom/Shop 1st Floor,Showroom/Shop 2nd Floor"</formula1>
+      <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,4+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="I2:I1048576">
       <formula1>"Advertise,Reference,99 Acres"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="K2:K1048576">
-      <formula1>"Thousand, Lac, Crore"</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="M2:M1048576">
-      <formula1>"Thousand, Lac, Crore"</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="N2:N1048576">
-      <formula1>"Rushil Pipaliya,lary Patel,test subhash test"</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="Q2:Q1048576">
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="L2:L1048576">
+      <formula1>"Admin Test,Bharat Makvana,dharmesh patel,dharmesh patel,raviraj chudasama,Nux Hathaliya,Nux Hathaliya"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="O2:O1048576">
       <formula1>"Active,In Active"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="R2:R1048576">
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="P2:P1048576">
       <formula1>"Lead Confirmed,Site Visit Scheduled,Site Visit Completed,Discussion,Booked,Lost"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Clone from live code
</commit_message>
<xml_diff>
--- a/public/imports/enquiry_sample.xlsx
+++ b/public/imports/enquiry_sample.xlsx
@@ -496,10 +496,10 @@
       <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,4+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="I2:I1048576">
-      <formula1>"Advertise,Reference,99 Acres,magicbricks,housing"</formula1>
+      <formula1>"Advertise,Reference,99 Acres"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="L2:L1048576">
-      <formula1>"bharat m"</formula1>
+      <formula1>"Admin Test,Bharat Makvana,dharmesh patel,dharmesh patel,raviraj chudasama,Nux Hathaliya,Nux Hathaliya"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="O2:O1048576">
       <formula1>"Active,In Active"</formula1>

</xml_diff>

<commit_message>
13-02 04-3 doc files
</commit_message>
<xml_diff>
--- a/public/imports/enquiry_sample.xlsx
+++ b/public/imports/enquiry_sample.xlsx
@@ -487,19 +487,19 @@
       <formula1>"Industrial,Commercial,Residential,Office &amp; Retail,Residential &amp; Commercial,Industrial,Residentia l&amp; Commercial,Industrial,Industrial,Industrial,Industrial"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="F2:F1048576">
-      <formula1>"Flat,Vila/Bunglow,Land/Plot,Penthouse,Farmhouse,Office,Retail,Storage/industrial,Plot/Land"</formula1>
+      <formula1>"Flat,Vila/Bunglow,Plot,Penthouse,Farmhouse,Office,Retail,Storage/industrial,Land"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="G2:G1048576">
-      <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,4+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
+      <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,5bhk,5+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="H2:H1048576">
-      <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,4+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
+      <formula1>"office space,Co-working,Ground floor,1st floor,2nd floor,3rd floor,Warehouse,Cold Storage,ind. shed,Commercial Land,Agricultural/Farm Land,Industrial Land,1 rk,1bhk,2bhk,3bhk,4bhk,5bhk,5+bhk,Plotting,1Bed,2Bed,3Bed,4Bed,4+Bed"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="I2:I1048576">
-      <formula1>"Advertise,Reference,99 Acres"</formula1>
+      <formula1>"Advertise,Reference,99 Acres,magicbricks,housing"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="L2:L1048576">
-      <formula1>"Admin Test,Bharat Makvana,dharmesh patel,dharmesh patel,raviraj chudasama,Nux Hathaliya,Nux Hathaliya"</formula1>
+      <formula1>"mr admin,chandresh patel,Amit Bharat Bhai"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Input error" error="Value is not in list." promptTitle="Pick from list" prompt="Please pick a value from the drop-down list." sqref="O2:O1048576">
       <formula1>"Active,In Active"</formula1>

</xml_diff>